<commit_message>
chore: remove legacy dashboard code and pages pipeline
</commit_message>
<xml_diff>
--- a/results/consolidated/Consolidated_NF_GARCH_Results.xlsx
+++ b/results/consolidated/Consolidated_NF_GARCH_Results.xlsx
@@ -12,11 +12,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
   <si>
+    <t xml:space="preserve">Model_Family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Engine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Split_Type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Source</t>
   </si>
   <si>
@@ -36,6 +45,15 @@
   </si>
   <si>
     <t xml:space="preserve">TGARCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GARCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TS_CV</t>
   </si>
   <si>
     <t xml:space="preserve">Time_Series_CV</t>
@@ -413,211 +431,301 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="n">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="n">
         <v>-6.23674331462475</v>
       </c>
-      <c r="D2" t="n">
+      <c r="G2" t="n">
         <v>-6.17773880124684</v>
       </c>
-      <c r="E2" t="n">
+      <c r="H2" t="n">
         <v>1566.18582865619</v>
       </c>
-      <c r="F2" t="n">
+      <c r="I2" t="n">
         <v>0.000265231788437081</v>
       </c>
-      <c r="G2" t="n">
+      <c r="J2" t="n">
         <v>0.00997959312049119</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="n">
-        <v>27401.3105107422</v>
-      </c>
-      <c r="D3" t="n">
-        <v>27439.8014735373</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-13694.6552553711</v>
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>-6.16499588686336</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>-6.10599137348545</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1548.24897171584</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.000265255247246037</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.00998057275133209</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
-        <v>-6.16499588686336</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-6.10599137348545</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1548.24897171584</v>
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
       </c>
       <c r="F4" t="n">
-        <v>0.000265255247246037</v>
+        <v>27401.3105107422</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00998057275133209</v>
+        <v>27439.8014735373</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-13694.6552553711</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="n">
         <v>-28273.7513163331</v>
       </c>
-      <c r="D5" t="n">
+      <c r="G5" t="n">
         <v>-28235.260353538</v>
       </c>
-      <c r="E5" t="n">
+      <c r="H5" t="n">
         <v>14142.8756581666</v>
       </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="n">
-        <v>-28244.7567895128</v>
-      </c>
-      <c r="D6" t="n">
-        <v>-28206.2658267177</v>
-      </c>
-      <c r="E6" t="n">
-        <v>14128.3783947564</v>
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>-6.23529221703763</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>-6.17628770365972</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1565.82305425941</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.000264427773901888</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.0099650836905736</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="n">
-        <v>-6.23529221703763</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-6.17628770365972</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1565.82305425941</v>
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
       </c>
       <c r="F7" t="n">
-        <v>0.000264427773901888</v>
+        <v>-28244.7567895128</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0099650836905736</v>
+        <v>-28206.2658267177</v>
+      </c>
+      <c r="H7" t="n">
+        <v>14128.3783947564</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="n">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="n">
         <v>-27993.3295905363</v>
       </c>
-      <c r="D8" t="n">
+      <c r="G8" t="n">
         <v>-27964.46136844</v>
       </c>
-      <c r="E8" t="n">
+      <c r="H8" t="n">
         <v>14001.1647952681</v>
       </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="n">
+      <c r="F9" t="n">
         <v>-6.14008516085673</v>
       </c>
-      <c r="D9" t="n">
+      <c r="G9" t="n">
         <v>-6.10636829606935</v>
       </c>
-      <c r="E9" t="n">
+      <c r="H9" t="n">
         <v>1539.02129021418</v>
       </c>
-      <c r="F9" t="n">
+      <c r="I9" t="n">
         <v>0.00026524306076551</v>
       </c>
-      <c r="G9" t="n">
+      <c r="J9" t="n">
         <v>0.00997754931432829</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="n">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="n">
         <v>-6.22901892609995</v>
       </c>
-      <c r="D10" t="n">
+      <c r="G10" t="n">
         <v>-6.17844362891889</v>
       </c>
-      <c r="E10" t="n">
+      <c r="H10" t="n">
         <v>1563.25473152499</v>
       </c>
-      <c r="F10" t="n">
+      <c r="I10" t="n">
         <v>0.000265218411076707</v>
       </c>
-      <c r="G10" t="n">
+      <c r="J10" t="n">
         <v>0.00997773042969076</v>
       </c>
     </row>

</xml_diff>